<commit_message>
update timesheet period april-may
</commit_message>
<xml_diff>
--- a/5_Period_20_Apr_2024_sd_19_May_2024/Timesheet Danamon-Bayu Bagus Bagaswara-April.xlsx
+++ b/5_Period_20_Apr_2024_sd_19_May_2024/Timesheet Danamon-Bayu Bagus Bagaswara-April.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\timesheet-danamon\5_Period_20_Apr_2024_sd_19_May_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\5_Period_20_Apr_2024_sd_19_May_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B99E18D-99D2-4FF5-974E-EF0D7A406E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C755934-5EB2-4044-99E3-4FF6DC10409F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -724,9 +724,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,7 +1114,7 @@
   <dimension ref="A1:EP23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
@@ -1515,10 +1512,10 @@
       <c r="AD9" s="61">
         <v>17</v>
       </c>
-      <c r="AE9" s="79">
+      <c r="AE9" s="61">
         <v>18</v>
       </c>
-      <c r="AF9" s="79">
+      <c r="AF9" s="61">
         <v>19</v>
       </c>
       <c r="AG9" s="46"/>
@@ -1757,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="T11" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" s="50">
         <v>2</v>
@@ -1785,7 +1782,7 @@
       <c r="AF11" s="56"/>
       <c r="AG11" s="44">
         <f>SUM(C11:AF11)</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH11" s="66"/>
       <c r="AI11" s="68"/>
@@ -1812,7 +1809,9 @@
       <c r="Q12" s="56"/>
       <c r="R12" s="56"/>
       <c r="S12" s="44"/>
-      <c r="T12" s="50"/>
+      <c r="T12" s="50">
+        <v>5</v>
+      </c>
       <c r="U12" s="50"/>
       <c r="V12" s="63"/>
       <c r="W12" s="63"/>
@@ -1827,7 +1826,7 @@
       <c r="AF12" s="56"/>
       <c r="AG12" s="44">
         <f>SUM(C12:AF12)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH12" s="66"/>
       <c r="AI12" s="68"/>
@@ -1875,7 +1874,7 @@
         <v>5</v>
       </c>
       <c r="T13" s="50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U13" s="50">
         <v>5</v>
@@ -1903,7 +1902,7 @@
       <c r="AF13" s="56"/>
       <c r="AG13" s="44">
         <f>SUM(C13:AF13)</f>
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AH13" s="66"/>
       <c r="AI13" s="68"/>

</xml_diff>